<commit_message>
in progress vumi flex
</commit_message>
<xml_diff>
--- a/Inputs/VUMI_Global_Flex/benefits.xlsx
+++ b/Inputs/VUMI_Global_Flex/benefits.xlsx
@@ -138,7 +138,7 @@
     <t xml:space="preserve">Diagnostics &amp; Test</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $deductible</t>
+    <t xml:space="preserve">Covered in full with $ deductible</t>
   </si>
   <si>
     <t xml:space="preserve">Surgeries &amp; Anesthesia</t>
@@ -150,7 +150,7 @@
     <t xml:space="preserve">Organ Transplant</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full including USD 50,000 for donor cost with $deductible</t>
+    <t xml:space="preserve">Covered in full including USD 50,000 for donor cost with $ deductible</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient (Consultations, Lab &amp; Diagnostics, Pharmacy, Physiotherapy)</t>
@@ -159,7 +159,7 @@
     <t xml:space="preserve">Out-patient Consultations</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $
+    <t xml:space="preserve">Covered in full with $ 
 </t>
   </si>
   <si>
@@ -172,22 +172,22 @@
     <t xml:space="preserve">Out-patient Medicines</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $</t>
+    <t xml:space="preserve">Covered in full with $ </t>
   </si>
   <si>
     <t xml:space="preserve">Vaccination</t>
   </si>
   <si>
-    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 500 with $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 350 with $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 250 with $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 150 with $</t>
+    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 500 with $ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 350 with $ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 250 with $ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel and preventive vaccinations covered up to USD 150 with $ </t>
   </si>
   <si>
     <t xml:space="preserve">Not Available</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">Physiotherapy</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $subject to pre-approval after 10 sessions
+    <t xml:space="preserve">Covered in full with $ subject to pre-approval after 10 sessions
 (Combined with Alternative medicines)</t>
   </si>
   <si>
@@ -287,14 +287,14 @@
     <t xml:space="preserve">Alternative Medicines</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $subject to pre-approval after 10 sessions
+    <t xml:space="preserve">Covered in full with $ subject to pre-approval after 10 sessions
 (Combined with Physiotherapy)</t>
   </si>
   <si>
     <t xml:space="preserve">Mental Health Benefit</t>
   </si>
   <si>
-    <t xml:space="preserve">OP Psychiatirc treatment covered up to USD 10,000 with $</t>
+    <t xml:space="preserve">OP Psychiatirc treatment covered up to USD 10,000 with $ </t>
   </si>
   <si>
     <t xml:space="preserve">Psychiatirc treatment covered up to USD 7,500</t>
@@ -817,10 +817,10 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83.66"/>

</xml_diff>